<commit_message>
Minor tweak to my_base.css.
</commit_message>
<xml_diff>
--- a/css_heading_sizes.xlsx
+++ b/css_heading_sizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\css_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E213016A-61CA-4885-84F3-63C38A1ABDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE63F7B-5681-41A4-B7D4-01B449883A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Heading</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>font-size: clamp();</t>
+  </si>
+  <si>
+    <t>h1-dbt</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -754,7 +757,7 @@
         <v>2.4000000000000004</v>
       </c>
       <c r="S3" s="13" t="str">
-        <f t="shared" ref="S3:S16" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
+        <f t="shared" ref="S3:S9" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
         <v>font-size: clamp(1.6rem, 1.2vw + 1rem, 2.4rem);</v>
       </c>
     </row>
@@ -818,7 +821,7 @@
         <v>33.6</v>
       </c>
       <c r="Q4" s="15">
-        <f t="shared" ref="Q4:Q7" si="7">D3*(K4/K3)</f>
+        <f t="shared" ref="Q4:Q6" si="7">D3*(K4/K3)</f>
         <v>1.4000000000000001</v>
       </c>
       <c r="R4" s="15">
@@ -1064,19 +1067,19 @@
         <v>0.8</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" ref="F8" si="10">IF(($F$1/100*B8/16)+C8&lt;D8,D8,IF(($F$1/100*B8/16)+C8&gt;J8,J8,($F$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="F8:F9" si="10">IF(($F$1/100*B8/16)+C8&lt;D8,D8,IF(($F$1/100*B8/16)+C8&gt;J8,J8,($F$1/100*B8/16)+C8))</f>
         <v>0.8</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" ref="G8" si="11">IF(($G$1/100*B8/16)+C8&lt;D8,D8,IF(($G$1/100*B8/16)+C8&gt;J8,J8,($G$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="G8:G9" si="11">IF(($G$1/100*B8/16)+C8&lt;D8,D8,IF(($G$1/100*B8/16)+C8&gt;J8,J8,($G$1/100*B8/16)+C8))</f>
         <v>0.85200000000000009</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" ref="H8" si="12">IF(($H$1/100*B8/16)+C8&lt;D8,D8,IF(($H$1/100*B8/16)+C8&gt;J8,J8,($H$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="H8:H9" si="12">IF(($H$1/100*B8/16)+C8&lt;D8,D8,IF(($H$1/100*B8/16)+C8&gt;J8,J8,($H$1/100*B8/16)+C8))</f>
         <v>0.9695625000000001</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" ref="I8" si="13">IF(($I$1/100*B8/16)+C8&lt;D8,D8,IF(($I$1/100*B8/16)+C8&gt;J8,J8,($I$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="I8:I9" si="13">IF(($I$1/100*B8/16)+C8&lt;D8,D8,IF(($I$1/100*B8/16)+C8&gt;J8,J8,($I$1/100*B8/16)+C8))</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="J8" s="10">
@@ -1086,23 +1089,23 @@
         <v>1</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" ref="L8" si="14">E8*16</f>
+        <f t="shared" ref="L8:L9" si="14">E8*16</f>
         <v>12.8</v>
       </c>
       <c r="M8" s="8">
-        <f t="shared" ref="M8" si="15">F8*16</f>
+        <f t="shared" ref="M8:M9" si="15">F8*16</f>
         <v>12.8</v>
       </c>
       <c r="N8" s="8">
-        <f t="shared" ref="N8" si="16">G8*16</f>
+        <f t="shared" ref="N8:N9" si="16">G8*16</f>
         <v>13.632000000000001</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" ref="O8" si="17">H8*16</f>
+        <f t="shared" ref="O8:O9" si="17">H8*16</f>
         <v>15.513000000000002</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" ref="P8" si="18">I8*16</f>
+        <f t="shared" ref="P8:P9" si="18">I8*16</f>
         <v>17.600000000000001</v>
       </c>
       <c r="Q8" s="16"/>
@@ -1113,25 +1116,70 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1.35</v>
+      </c>
+      <c r="E9" s="4">
+        <f>IF(($E$1/100*B9/16)+C9&lt;D9,D9,IF(($E$1/100*B9/16)+C9&gt;J9,J9,($E$1/100*B9/16)+C9))</f>
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="10"/>
+        <v>1.8399999999999999</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="11"/>
+        <v>2.12</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="12"/>
+        <v>2.4940625000000001</v>
+      </c>
+      <c r="I9" s="4">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="J9" s="10">
+        <v>3</v>
+      </c>
+      <c r="K9" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="14"/>
+        <v>24.4</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="15"/>
+        <v>29.439999999999998</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="16"/>
+        <v>33.92</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="17"/>
+        <v>39.905000000000001</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="18"/>
+        <v>48</v>
+      </c>
       <c r="Q9" s="17"/>
       <c r="R9" s="16"/>
-      <c r="S9" s="13"/>
+      <c r="S9" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>font-size: clamp(1.35rem, 1.75vw + 1rem, 3rem);</v>
+      </c>
     </row>
     <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>

</xml_diff>

<commit_message>
Added a couple rows to css_heading_styles.xlsx.
</commit_message>
<xml_diff>
--- a/css_heading_sizes.xlsx
+++ b/css_heading_sizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\code\css_modules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\css_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049746C5-4751-438B-B662-77F278A6AD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A81DDE-3322-4FD9-94CF-08ABE9F6D627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Heading</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>h1-dbt</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>text3</t>
   </si>
 </sst>
 </file>
@@ -176,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -194,9 +200,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,16 +220,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,20 +543,19 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.69921875" style="2"/>
-    <col min="2" max="11" width="8.69921875" style="3"/>
-    <col min="12" max="17" width="8.69921875" style="1"/>
-    <col min="18" max="18" width="9.09765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.09765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.69921875" style="1"/>
+    <col min="1" max="1" width="8.75" style="2"/>
+    <col min="2" max="17" width="8.75" style="3"/>
+    <col min="18" max="18" width="9.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -572,19 +568,19 @@
       <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7">
+      <c r="E1" s="6">
         <v>480</v>
       </c>
-      <c r="F1" s="7">
+      <c r="F1" s="6">
         <v>768</v>
       </c>
-      <c r="G1" s="7">
+      <c r="G1" s="6">
         <v>1024</v>
       </c>
-      <c r="H1" s="7">
+      <c r="H1" s="6">
         <v>1366</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="6">
         <v>1920</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -593,32 +589,32 @@
       <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="6">
         <v>480</v>
       </c>
-      <c r="M1" s="7">
+      <c r="M1" s="6">
         <v>768</v>
       </c>
-      <c r="N1" s="7">
+      <c r="N1" s="6">
         <v>1024</v>
       </c>
-      <c r="O1" s="7">
+      <c r="O1" s="6">
         <v>1366</v>
       </c>
-      <c r="P1" s="7">
+      <c r="P1" s="6">
         <v>1920</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -628,7 +624,7 @@
       <c r="C2" s="4">
         <v>1.25</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>2</v>
       </c>
       <c r="E2" s="4">
@@ -651,45 +647,45 @@
         <f>IF(($I$1/100*B2/16)+C2&lt;D2,D2,IF(($I$1/100*B2/16)+C2&gt;J2,J2,($I$1/100*B2/16)+C2))</f>
         <v>3</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="9">
         <v>3</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>2.5</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <f>E2*16</f>
         <v>32</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="7">
         <f t="shared" ref="M2:P7" si="0">F2*16</f>
         <v>32</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="7">
         <f t="shared" si="0"/>
         <v>35.36</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="7">
         <f t="shared" si="0"/>
         <v>40.49</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="7">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="13">
         <v>2</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="13">
         <f>J2</f>
         <v>3</v>
       </c>
-      <c r="S2" s="13" t="str">
+      <c r="S2" s="12" t="str">
         <f>"font-size: clamp("&amp;D2&amp;"rem, "&amp;B2&amp;"vw + "&amp;C2&amp;"rem, "&amp;J2&amp;"rem);"</f>
         <v>font-size: clamp(2rem, 1.5vw + 1.25rem, 3rem);</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -699,7 +695,7 @@
       <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1.6</v>
       </c>
       <c r="E3" s="4">
@@ -722,46 +718,46 @@
         <f t="shared" ref="I3:I7" si="4">IF(($I$1/100*B3/16)+C3&lt;D3,D3,IF(($I$1/100*B3/16)+C3&gt;J3,J3,($I$1/100*B3/16)+C3))</f>
         <v>2.4</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="9">
         <v>2.4</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="8">
         <v>2</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="7">
         <f t="shared" ref="L3:L7" si="5">E3*16</f>
         <v>25.6</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="7">
         <f t="shared" si="0"/>
         <v>25.6</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <f t="shared" si="0"/>
         <v>28.288</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <f t="shared" si="0"/>
         <v>32.391999999999996</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="7">
         <f t="shared" si="0"/>
         <v>38.4</v>
       </c>
-      <c r="Q3" s="15">
+      <c r="Q3" s="13">
         <f>D2*(K3/K2)</f>
         <v>1.6</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="13">
         <f>J2*(K3/K2)</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="S3" s="13" t="str">
-        <f t="shared" ref="S3:S10" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
+      <c r="S3" s="12" t="str">
+        <f t="shared" ref="S3:S11" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
         <v>font-size: clamp(1.6rem, 1.2vw + 1rem, 2.4rem);</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -771,7 +767,7 @@
       <c r="C4" s="4">
         <v>0.9</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>1.4</v>
       </c>
       <c r="E4" s="4">
@@ -794,46 +790,46 @@
         <f t="shared" si="4"/>
         <v>2.1</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>2.1</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <v>1.75</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <f t="shared" si="5"/>
         <v>22.4</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="7">
         <f t="shared" si="0"/>
         <v>22.4</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <f t="shared" si="0"/>
         <v>24.64</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <f t="shared" si="0"/>
         <v>28.060000000000002</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="7">
         <f t="shared" si="0"/>
         <v>33.6</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="13">
         <f t="shared" ref="Q4:Q6" si="7">D3*(K4/K3)</f>
         <v>1.4000000000000001</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="13">
         <f>J3*(K4/K3)</f>
         <v>2.1</v>
       </c>
-      <c r="S4" s="13" t="str">
+      <c r="S4" s="12" t="str">
         <f t="shared" si="6"/>
         <v>font-size: clamp(1.4rem, 1vw + 0.9rem, 2.1rem);</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -843,7 +839,7 @@
       <c r="C5" s="4">
         <v>0.8</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>1.2</v>
       </c>
       <c r="E5" s="4">
@@ -866,46 +862,46 @@
         <f t="shared" si="4"/>
         <v>1.8</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="9">
         <v>1.8</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>1.5</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="7">
         <f t="shared" si="5"/>
         <v>19.2</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="7">
         <f t="shared" si="0"/>
         <v>19.327999999999999</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <f t="shared" si="0"/>
         <v>21.504000000000001</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="7">
         <f t="shared" si="0"/>
         <v>24.411000000000001</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="7">
         <f t="shared" si="0"/>
         <v>28.8</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="13">
         <f t="shared" si="7"/>
         <v>1.2</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="13">
         <f t="shared" ref="R5:R7" si="9">J4*(K5/K4)</f>
         <v>1.8</v>
       </c>
-      <c r="S5" s="13" t="str">
+      <c r="S5" s="12" t="str">
         <f t="shared" si="6"/>
         <v>font-size: clamp(1.2rem, 0.85vw + 0.8rem, 1.8rem);</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -915,7 +911,7 @@
       <c r="C6" s="4">
         <v>0.7</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" s="4">
@@ -938,46 +934,46 @@
         <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>1.5</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <v>1.25</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <f t="shared" si="5"/>
         <v>17.600000000000001</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <f t="shared" si="0"/>
         <v>17.600000000000001</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <f t="shared" si="0"/>
         <v>18.367999999999999</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <f t="shared" si="0"/>
         <v>20.762</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="13">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="13">
         <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
-      <c r="S6" s="13" t="str">
+      <c r="S6" s="12" t="str">
         <f t="shared" si="6"/>
         <v>font-size: clamp(1.1rem, 0.7vw + 0.7rem, 1.5rem);</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -987,7 +983,7 @@
       <c r="C7" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="4">
@@ -1010,46 +1006,46 @@
         <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="9">
         <v>1.2</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="8">
         <v>1</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="7">
         <f t="shared" si="0"/>
         <v>16.313000000000002</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="7">
         <f t="shared" si="0"/>
         <v>19.2</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="13">
         <f>D6*(K7/K6)</f>
         <v>0.88000000000000012</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="13">
         <f t="shared" si="9"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="S7" s="13" t="str">
+      <c r="S7" s="12" t="str">
         <f t="shared" si="6"/>
         <v>font-size: clamp(1rem, 0.55vw + 0.55rem, 1.2rem);</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1059,7 +1055,7 @@
       <c r="C8" s="4">
         <v>0.5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.8</v>
       </c>
       <c r="E8" s="4">
@@ -1067,55 +1063,55 @@
         <v>0.8</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" ref="F8:F10" si="10">IF(($F$1/100*B8/16)+C8&lt;D8,D8,IF(($F$1/100*B8/16)+C8&gt;J8,J8,($F$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="F8:F9" si="10">IF(($F$1/100*B8/16)+C8&lt;D8,D8,IF(($F$1/100*B8/16)+C8&gt;J8,J8,($F$1/100*B8/16)+C8))</f>
         <v>0.8</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" ref="G8:G10" si="11">IF(($G$1/100*B8/16)+C8&lt;D8,D8,IF(($G$1/100*B8/16)+C8&gt;J8,J8,($G$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="G8:G9" si="11">IF(($G$1/100*B8/16)+C8&lt;D8,D8,IF(($G$1/100*B8/16)+C8&gt;J8,J8,($G$1/100*B8/16)+C8))</f>
         <v>0.85200000000000009</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" ref="H8:H10" si="12">IF(($H$1/100*B8/16)+C8&lt;D8,D8,IF(($H$1/100*B8/16)+C8&gt;J8,J8,($H$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="H8:H9" si="12">IF(($H$1/100*B8/16)+C8&lt;D8,D8,IF(($H$1/100*B8/16)+C8&gt;J8,J8,($H$1/100*B8/16)+C8))</f>
         <v>0.9695625000000001</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" ref="I8:I10" si="13">IF(($I$1/100*B8/16)+C8&lt;D8,D8,IF(($I$1/100*B8/16)+C8&gt;J8,J8,($I$1/100*B8/16)+C8))</f>
+        <f t="shared" ref="I8:I9" si="13">IF(($I$1/100*B8/16)+C8&lt;D8,D8,IF(($I$1/100*B8/16)+C8&gt;J8,J8,($I$1/100*B8/16)+C8))</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="8">
         <v>1</v>
       </c>
-      <c r="L8" s="8">
-        <f t="shared" ref="L8:L10" si="14">E8*16</f>
+      <c r="L8" s="7">
+        <f t="shared" ref="L8:L9" si="14">E8*16</f>
         <v>12.8</v>
       </c>
-      <c r="M8" s="8">
-        <f t="shared" ref="M8:M10" si="15">F8*16</f>
+      <c r="M8" s="7">
+        <f t="shared" ref="M8:M9" si="15">F8*16</f>
         <v>12.8</v>
       </c>
-      <c r="N8" s="8">
-        <f t="shared" ref="N8:N10" si="16">G8*16</f>
+      <c r="N8" s="7">
+        <f t="shared" ref="N8:N9" si="16">G8*16</f>
         <v>13.632000000000001</v>
       </c>
-      <c r="O8" s="8">
-        <f t="shared" ref="O8:O10" si="17">H8*16</f>
+      <c r="O8" s="7">
+        <f t="shared" ref="O8:O9" si="17">H8*16</f>
         <v>15.513000000000002</v>
       </c>
-      <c r="P8" s="8">
-        <f t="shared" ref="P8:P10" si="18">I8*16</f>
+      <c r="P8" s="7">
+        <f t="shared" ref="P8:P9" si="18">I8*16</f>
         <v>17.600000000000001</v>
       </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="13" t="str">
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="12" t="str">
         <f t="shared" si="6"/>
         <v>font-size: clamp(0.8rem, 0.55vw + 0.5rem, 1.1rem);</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1125,7 +1121,7 @@
       <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>1.35</v>
       </c>
       <c r="E9" s="4">
@@ -1148,185 +1144,275 @@
         <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="9">
         <v>3</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>2.5</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="7">
         <f t="shared" si="14"/>
         <v>24.4</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="7">
         <f t="shared" si="15"/>
         <v>29.439999999999998</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="7">
         <f t="shared" si="16"/>
         <v>33.92</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="7">
         <f t="shared" si="17"/>
         <v>39.905000000000001</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="7">
         <f t="shared" si="18"/>
         <v>48</v>
       </c>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="13" t="str">
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="12" t="str">
         <f t="shared" si="6"/>
         <v>font-size: clamp(1.35rem, 1.75vw + 1rem, 3rem);</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="13"/>
-    </row>
-    <row r="11" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="13"/>
-    </row>
-    <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" ref="E10:E11" si="19">IF(($E$1/100*B10/16)+C10&lt;D10,D10,IF(($E$1/100*B10/16)+C10&gt;J10,J10,($E$1/100*B10/16)+C10))</f>
+        <v>0.9</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" ref="F10:F11" si="20">IF(($F$1/100*B10/16)+C10&lt;D10,D10,IF(($F$1/100*B10/16)+C10&gt;J10,J10,($F$1/100*B10/16)+C10))</f>
+        <v>0.9</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" ref="G10:G11" si="21">IF(($G$1/100*B10/16)+C10&lt;D10,D10,IF(($G$1/100*B10/16)+C10&gt;J10,J10,($G$1/100*B10/16)+C10))</f>
+        <v>0.90200000000000014</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" ref="H10:H11" si="22">IF(($H$1/100*B10/16)+C10&lt;D10,D10,IF(($H$1/100*B10/16)+C10&gt;J10,J10,($H$1/100*B10/16)+C10))</f>
+        <v>1.0195625000000001</v>
+      </c>
+      <c r="I10" s="4">
+        <f t="shared" ref="I10:I11" si="23">IF(($I$1/100*B10/16)+C10&lt;D10,D10,IF(($I$1/100*B10/16)+C10&gt;J10,J10,($I$1/100*B10/16)+C10))</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" ref="L10:L11" si="24">E10*16</f>
+        <v>14.4</v>
+      </c>
+      <c r="M10" s="7">
+        <f t="shared" ref="M10:M11" si="25">F10*16</f>
+        <v>14.4</v>
+      </c>
+      <c r="N10" s="7">
+        <f t="shared" ref="N10:N11" si="26">G10*16</f>
+        <v>14.432000000000002</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" ref="O10:O11" si="27">H10*16</f>
+        <v>16.313000000000002</v>
+      </c>
+      <c r="P10" s="7">
+        <f t="shared" ref="P10:P11" si="28">I10*16</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>font-size: clamp(0.9rem, 0.55vw + 0.55rem, 1.1rem);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="19"/>
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="21"/>
+        <v>0.85200000000000009</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="22"/>
+        <v>0.9695625000000001</v>
+      </c>
+      <c r="I11" s="4">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="24"/>
+        <v>12.8</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="25"/>
+        <v>12.8</v>
+      </c>
+      <c r="N11" s="7">
+        <f t="shared" si="26"/>
+        <v>13.632000000000001</v>
+      </c>
+      <c r="O11" s="7">
+        <f t="shared" si="27"/>
+        <v>15.513000000000002</v>
+      </c>
+      <c r="P11" s="7">
+        <f t="shared" si="28"/>
+        <v>16</v>
+      </c>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>font-size: clamp(0.8rem, 0.55vw + 0.5rem, 1rem);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="10"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="13"/>
-    </row>
-    <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="9"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="12"/>
+    </row>
+    <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="10"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="13"/>
-    </row>
-    <row r="14" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="9"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="12"/>
+    </row>
+    <row r="14" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="13"/>
-    </row>
-    <row r="15" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="9"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="12"/>
+    </row>
+    <row r="15" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="10"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="13"/>
-    </row>
-    <row r="16" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="9"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="12"/>
+    </row>
+    <row r="16" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="13"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Made an addition to css_heading_sizes.xlsx.
</commit_message>
<xml_diff>
--- a/css_heading_sizes.xlsx
+++ b/css_heading_sizes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\css_modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A81DDE-3322-4FD9-94CF-08ABE9F6D627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337E7743-8F48-4984-BD88-A3A62AC08527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F820B3DE-D05A-4853-9D82-A8DA71430E49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Heading</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>text3</t>
+  </si>
+  <si>
+    <t>text4</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -753,7 +756,7 @@
         <v>2.4000000000000004</v>
       </c>
       <c r="S3" s="12" t="str">
-        <f t="shared" ref="S3:S11" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
+        <f t="shared" ref="S3:S12" si="6">"font-size: clamp("&amp;D3&amp;"rem, "&amp;B3&amp;"vw + "&amp;C3&amp;"rem, "&amp;J3&amp;"rem);"</f>
         <v>font-size: clamp(1.6rem, 1.2vw + 1rem, 2.4rem);</v>
       </c>
     </row>
@@ -1310,25 +1313,70 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" ref="E12" si="29">IF(($E$1/100*B12/16)+C12&lt;D12,D12,IF(($E$1/100*B12/16)+C12&gt;J12,J12,($E$1/100*B12/16)+C12))</f>
+        <v>0.9</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" ref="F12" si="30">IF(($F$1/100*B12/16)+C12&lt;D12,D12,IF(($F$1/100*B12/16)+C12&gt;J12,J12,($F$1/100*B12/16)+C12))</f>
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" ref="G12" si="31">IF(($G$1/100*B12/16)+C12&lt;D12,D12,IF(($G$1/100*B12/16)+C12&gt;J12,J12,($G$1/100*B12/16)+C12))</f>
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" ref="H12" si="32">IF(($H$1/100*B12/16)+C12&lt;D12,D12,IF(($H$1/100*B12/16)+C12&gt;J12,J12,($H$1/100*B12/16)+C12))</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" ref="I12" si="33">IF(($I$1/100*B12/16)+C12&lt;D12,D12,IF(($I$1/100*B12/16)+C12&gt;J12,J12,($I$1/100*B12/16)+C12))</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="9">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" ref="L12" si="34">E12*16</f>
+        <v>14.4</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" ref="M12" si="35">F12*16</f>
+        <v>14.4</v>
+      </c>
+      <c r="N12" s="7">
+        <f t="shared" ref="N12" si="36">G12*16</f>
+        <v>15.231999999999999</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" ref="O12" si="37">H12*16</f>
+        <v>16</v>
+      </c>
+      <c r="P12" s="7">
+        <f t="shared" ref="P12" si="38">I12*16</f>
+        <v>16</v>
+      </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
-      <c r="S12" s="12"/>
+      <c r="S12" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v>font-size: clamp(0.9rem, 0.55vw + 0.6rem, 1rem);</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>

</xml_diff>